<commit_message>
add cartonid is list for asn
</commit_message>
<xml_diff>
--- a/FrmPIE/0temple/templesforASNDefault.xlsx
+++ b/FrmPIE/0temple/templesforASNDefault.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20550" windowHeight="3990"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="23715" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="e-Pack ver 5 (0317)" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Customer purchase order no.</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -657,13 +657,13 @@
         <v>14</v>
       </c>
       <c r="F3" s="7">
-        <v>54000</v>
+        <v>10000</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="7">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="I3" s="7">
         <v>1</v>
@@ -676,207 +676,377 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8">
-        <v>10749337</v>
+        <v>10749336</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4" s="7">
-        <v>130000</v>
+        <v>10000</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B5" s="8">
-        <v>10750334</v>
+        <v>10749336</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F5" s="7">
-        <v>3000</v>
+        <v>10000</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H5" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B6" s="8">
-        <v>10751282</v>
+        <v>10749336</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F6" s="7">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="H6" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B7" s="8">
-        <v>10752298</v>
+        <v>10749336</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F7" s="7">
-        <v>4000</v>
+        <v>10000</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H7" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="7" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B8" s="8">
-        <v>10757109</v>
+        <v>10749336</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="F8" s="7">
-        <v>14000</v>
+        <v>4000</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="H8" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I8" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8">
-        <v>10750167</v>
+        <v>10749337</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7">
-        <v>2000</v>
+        <v>130000</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
       </c>
       <c r="I9" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="8">
+        <v>10750334</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="7">
+        <v>3000</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>2</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10751282</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="7">
+        <v>60000</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7">
+        <v>2</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8">
+        <v>10752298</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4000</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8">
+        <v>10757109</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7">
+        <v>14000</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7">
+        <v>3</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="8">
+        <v>10750167</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7">
+        <v>3</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>